<commit_message>
thay đổi về database
thêm 5 cột result và result các agents vào bảng s_flow
thay đổi bảng database -> trustedDatabase
thêm bảng threatsDatabase
</commit_message>
<xml_diff>
--- a/database.xlsx
+++ b/database.xlsx
@@ -6,7 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="database" r:id="rId3" sheetId="1"/>
+    <sheet name="threats_database" r:id="rId3" sheetId="1"/>
+    <sheet name="trusted_database" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
@@ -49,8 +50,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -81,12 +85,49 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>192.168.10.1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>1.1.1.1.1.1</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>src ip</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>src mac</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
           <t>1.2.3.4</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>10:10:10:10:10:10</t>
+          <t>10.10.10.10.10.10</t>
         </is>
       </c>
     </row>

</xml_diff>